<commit_message>
Finalizada a planilha com todo o dicionario de dados.
</commit_message>
<xml_diff>
--- a/documentos/Dicionario_de_dados_planilha.xlsx
+++ b/documentos/Dicionario_de_dados_planilha.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="0" yWindow="75" windowWidth="38355" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="TODAS_VARIAVEIS" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TODAS_VARIAVEIS!$A$1:$F$45</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="852">
   <si>
     <t>Nome do Campo</t>
   </si>
@@ -2035,6 +2035,546 @@
   </si>
   <si>
     <t>DS_AN_OUT</t>
+  </si>
+  <si>
+    <t>68-Laboratório que realizou o Teste antigênico (CNES)</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico que foi positivo para Influenza</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico, para o tipo de Influenza.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico, que foi positivo para outro vírus respiratório.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico, para SARS-CoV-2.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico, para VSR.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico, para Parainfluenza 1.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico. Parainfluenza 2</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico. Parainfluenza 3</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico. Adenovírus.</t>
+  </si>
+  <si>
+    <t>Resultado do Teste Antigênico.Outro vírus respiratório</t>
+  </si>
+  <si>
+    <t>Nome do outro vírus respiratório identificado pelo Teste Antigênico.</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>70-Resultado da RT-PCR/outro método por Biologia Molecular</t>
+  </si>
+  <si>
+    <t>PCR_RESUL</t>
+  </si>
+  <si>
+    <t>Resultado do teste de RT-PCR/outro método por Biologia Molecular</t>
+  </si>
+  <si>
+    <t>71-Data do Resultado RT-PCR/outro método por Biologia Molecular</t>
+  </si>
+  <si>
+    <t>DT_PCR</t>
+  </si>
+  <si>
+    <t>Data do Resultado RT-PCR/outro método por Biologia Molecular</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Positivo para Influenza?</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Se sim, qual Influenza?</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Se Influenza A, qual subtipo?</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Se Influenza A, qual subtipo? Outro, especifique:</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Se Influenza B, qual linhagem?</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Se Influenza B, qual linhagem? Outro, especifique:</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Positivo para outros vírus?</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: SARS-CoV-2</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: VSR</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Parainfluenza 1</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Parainfluenza 2</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Parainfluenza 3</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Parainfluenza 4</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Adenovírus</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Metapneumovírus</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Bocavírus</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Rinovírus</t>
+  </si>
+  <si>
+    <t>72- Agente etiológico – RT-PCR/outro método por Biologia Molecular: Outro vírus respiratório, especifique:</t>
+  </si>
+  <si>
+    <t>POS_PCRFLU</t>
+  </si>
+  <si>
+    <t>TP_FLU_PCR</t>
+  </si>
+  <si>
+    <t>PCR_FLUASU</t>
+  </si>
+  <si>
+    <t>FLUASU_OUT</t>
+  </si>
+  <si>
+    <t>PCR_FLUBLI</t>
+  </si>
+  <si>
+    <t>FLUBLI_OUT</t>
+  </si>
+  <si>
+    <t>POS_PCROUT</t>
+  </si>
+  <si>
+    <t>PCR_ SARS2</t>
+  </si>
+  <si>
+    <t>PCR_VSR</t>
+  </si>
+  <si>
+    <t>PCR_PARA1</t>
+  </si>
+  <si>
+    <t>PCR_PARA2</t>
+  </si>
+  <si>
+    <t>PCR_PARA3</t>
+  </si>
+  <si>
+    <t>PCR_PARA4</t>
+  </si>
+  <si>
+    <t>PCR_ADENO</t>
+  </si>
+  <si>
+    <t>PCR_METAP</t>
+  </si>
+  <si>
+    <t>PCR_BOCA</t>
+  </si>
+  <si>
+    <t>PCR_RINO</t>
+  </si>
+  <si>
+    <t>PCR_OUTRO</t>
+  </si>
+  <si>
+    <t>DS_PCR_OUT</t>
+  </si>
+  <si>
+    <t>Resultado da RTPCR foi positivo para Influenza</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para o tipo de Influenza.</t>
+  </si>
+  <si>
+    <t>Subtipo para Influenza A.</t>
+  </si>
+  <si>
+    <t>Outro subtipo para Influenza A.</t>
+  </si>
+  <si>
+    <t>Linhagem para Influenza B.</t>
+  </si>
+  <si>
+    <t>Outra linhagem para Influenza B</t>
+  </si>
+  <si>
+    <t>Resultado da RTPCR foi positivo para outro vírus respiratório</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para (SARS-CoV2).</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para (VSR).</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Parainfluenza 1.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Parainfluenza 2.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Parainfluenza 3.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Parainfluenza 4.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Adenovírus.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Metapneumovírus.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Bocavírus.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Rinovírus.</t>
+  </si>
+  <si>
+    <t>Resultado diagnóstico do RTPCR para Outro vírus respiratório.</t>
+  </si>
+  <si>
+    <t>Nome do outro vírus respiratório identificado pelo RT-PCR.</t>
+  </si>
+  <si>
+    <t>73-Laboratório que realizou RTPCR/outro método por Biologia Molecular Código (CNES)</t>
+  </si>
+  <si>
+    <t>Laboratório responsável pela liberação do resultado do teste diagnóstico (RTPCR) da amostra do paciente</t>
+  </si>
+  <si>
+    <t>LAB_PCR</t>
+  </si>
+  <si>
+    <t>CO_LAB_PCR</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>74- Tipo de Amostra Sorológica para SARS-Cov-2</t>
+  </si>
+  <si>
+    <t>Tipo de amostra sorológica que foi coletada</t>
+  </si>
+  <si>
+    <t>TP_AM_SOR</t>
+  </si>
+  <si>
+    <t>Tipo de Amostra Sorológica para SARSCov-2/Outra, qual?</t>
+  </si>
+  <si>
+    <t>SOR_OUT</t>
+  </si>
+  <si>
+    <t>Descrição do tipo da amostra clínica, caso diferente das listadas na categoria um (1) do campo.</t>
+  </si>
+  <si>
+    <t>75- Data da coleta</t>
+  </si>
+  <si>
+    <t>DT_CO_SOR</t>
+  </si>
+  <si>
+    <t>Data da coleta do material para diagnóstico por Sorologia.</t>
+  </si>
+  <si>
+    <t>76- Tipo de Sorologia para SARS-Cov-2</t>
+  </si>
+  <si>
+    <t>Tipo do Teste Sorológico que foi realizado</t>
+  </si>
+  <si>
+    <t>TP_SOR</t>
+  </si>
+  <si>
+    <t>Descrição do tipo de Teste Sorológico</t>
+  </si>
+  <si>
+    <t>OUT_SOR</t>
+  </si>
+  <si>
+    <t>76- Tipo de Sorologia para SARS-Cov2/Outro, qual?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76- Resultado do Teste Sorológico para SARS-CoV-2: </t>
+  </si>
+  <si>
+    <t>76- Resultado do Teste Sorológico para SARS-CoV-2:</t>
+  </si>
+  <si>
+    <t>RES_IGA</t>
+  </si>
+  <si>
+    <t>Resultado da Sorologia para SARS-CoV-2</t>
+  </si>
+  <si>
+    <t>RES_IGM</t>
+  </si>
+  <si>
+    <t>RES_IGG</t>
+  </si>
+  <si>
+    <t>Outro tipo de amostra Sorológica</t>
+  </si>
+  <si>
+    <t>77- Data do Resultado</t>
+  </si>
+  <si>
+    <t>Data do Resultado do Teste Sorológico</t>
+  </si>
+  <si>
+    <t>DT_RES</t>
+  </si>
+  <si>
+    <t>78-Classificação final do caso</t>
+  </si>
+  <si>
+    <t>Diagnóstico final do caso. Se tiver resultados divergentes entre as metodologias laboratoriais, priorizar o resultado do RTPCR.</t>
+  </si>
+  <si>
+    <t>CLASSI_FIN</t>
+  </si>
+  <si>
+    <t>78-Classificação final do caso 3-SRAG por outra causa , qual:</t>
+  </si>
+  <si>
+    <t>CLASSI_OUT</t>
+  </si>
+  <si>
+    <t>Descrição de qual outro agente etiológico foi identificado</t>
+  </si>
+  <si>
+    <t>79–Critério de Encerramento</t>
+  </si>
+  <si>
+    <t>Indicar qual o critério de confirmação</t>
+  </si>
+  <si>
+    <t>CRITERIO</t>
+  </si>
+  <si>
+    <t>80–Evolução do caso</t>
+  </si>
+  <si>
+    <t>Evolução do caso</t>
+  </si>
+  <si>
+    <t>EVOLUCAO</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>81–Data da alta ou óbito</t>
+  </si>
+  <si>
+    <t>Data da alta ou óbito</t>
+  </si>
+  <si>
+    <t>DT_EVOLUCA</t>
+  </si>
+  <si>
+    <t>82-Data do Encerramento</t>
+  </si>
+  <si>
+    <t>DT_ENCERRA</t>
+  </si>
+  <si>
+    <t>Data do encerramento do caso.</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>83- Número D.O</t>
+  </si>
+  <si>
+    <t>NU_DO</t>
+  </si>
+  <si>
+    <t>Número da Declaração de Óbito</t>
+  </si>
+  <si>
+    <t>84-Observações</t>
+  </si>
+  <si>
+    <t>Outras observações sobre o paciente consideradas pertinentes.</t>
+  </si>
+  <si>
+    <t>OBSERVA</t>
+  </si>
+  <si>
+    <t>85-Profissional de Saúde Responsável</t>
+  </si>
+  <si>
+    <t>Nome completo do profissional de saúde (sem abreviações) responsável pela notificação.</t>
+  </si>
+  <si>
+    <t>NOME_PROF</t>
+  </si>
+  <si>
+    <t>86-Registro Conselho/Matrícula</t>
+  </si>
+  <si>
+    <t>REG_PROF</t>
+  </si>
+  <si>
+    <t>Número do conselho ou matrícula do profissional de saúde responsável pela notificação (Ex: CRM/RJ 1234)</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>Data da digitação</t>
+  </si>
+  <si>
+    <t>DT_DIGITA</t>
+  </si>
+  <si>
+    <t>Data de inclusão do registro no sistema</t>
   </si>
 </sst>
 </file>
@@ -2411,18 +2951,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="168" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="116.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -5107,7 +5647,7 @@
         <v>634</v>
       </c>
       <c r="B137" t="s">
-        <v>638</v>
+        <v>672</v>
       </c>
       <c r="C137" t="s">
         <v>640</v>
@@ -5126,6 +5666,9 @@
       <c r="C138" t="s">
         <v>661</v>
       </c>
+      <c r="D138" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
@@ -5137,6 +5680,9 @@
       <c r="C139" t="s">
         <v>662</v>
       </c>
+      <c r="D139" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
@@ -5148,6 +5694,9 @@
       <c r="C140" t="s">
         <v>663</v>
       </c>
+      <c r="D140" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
@@ -5159,6 +5708,9 @@
       <c r="C141" t="s">
         <v>664</v>
       </c>
+      <c r="D141" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
@@ -5170,6 +5722,9 @@
       <c r="C142" t="s">
         <v>665</v>
       </c>
+      <c r="D142" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
@@ -5181,6 +5736,9 @@
       <c r="C143" t="s">
         <v>666</v>
       </c>
+      <c r="D143" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
@@ -5192,8 +5750,11 @@
       <c r="C144" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="D144" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="4" t="s">
         <v>657</v>
       </c>
@@ -5203,8 +5764,11 @@
       <c r="C145" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="D145" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="4" t="s">
         <v>658</v>
       </c>
@@ -5214,8 +5778,11 @@
       <c r="C146" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="D146" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="4" t="s">
         <v>659</v>
       </c>
@@ -5225,8 +5792,11 @@
       <c r="C147" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="148" spans="1:3">
+      <c r="D147" s="7" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="4" t="s">
         <v>660</v>
       </c>
@@ -5236,6 +5806,631 @@
       <c r="C148" t="s">
         <v>671</v>
       </c>
+      <c r="D148" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="B149" t="s">
+        <v>699</v>
+      </c>
+      <c r="C149" t="s">
+        <v>700</v>
+      </c>
+      <c r="D149" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="B150" t="s">
+        <v>702</v>
+      </c>
+      <c r="C150" t="s">
+        <v>703</v>
+      </c>
+      <c r="D150" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="B151" t="s">
+        <v>705</v>
+      </c>
+      <c r="C151" t="s">
+        <v>730</v>
+      </c>
+      <c r="D151" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="B152" t="s">
+        <v>706</v>
+      </c>
+      <c r="C152" t="s">
+        <v>731</v>
+      </c>
+      <c r="D152" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="B153" t="s">
+        <v>707</v>
+      </c>
+      <c r="C153" t="s">
+        <v>732</v>
+      </c>
+      <c r="D153" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="B154" t="s">
+        <v>708</v>
+      </c>
+      <c r="C154" t="s">
+        <v>733</v>
+      </c>
+      <c r="D154" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="B155" t="s">
+        <v>709</v>
+      </c>
+      <c r="C155" t="s">
+        <v>734</v>
+      </c>
+      <c r="D155" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="B156" t="s">
+        <v>710</v>
+      </c>
+      <c r="C156" t="s">
+        <v>735</v>
+      </c>
+      <c r="D156" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="B157" t="s">
+        <v>711</v>
+      </c>
+      <c r="C157" t="s">
+        <v>736</v>
+      </c>
+      <c r="D157" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="B158" t="s">
+        <v>712</v>
+      </c>
+      <c r="C158" t="s">
+        <v>737</v>
+      </c>
+      <c r="D158" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="B159" t="s">
+        <v>713</v>
+      </c>
+      <c r="C159" t="s">
+        <v>738</v>
+      </c>
+      <c r="D159" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="B160" t="s">
+        <v>714</v>
+      </c>
+      <c r="C160" t="s">
+        <v>739</v>
+      </c>
+      <c r="D160" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="B161" t="s">
+        <v>715</v>
+      </c>
+      <c r="C161" t="s">
+        <v>740</v>
+      </c>
+      <c r="D161" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="B162" t="s">
+        <v>716</v>
+      </c>
+      <c r="C162" t="s">
+        <v>741</v>
+      </c>
+      <c r="D162" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="B163" t="s">
+        <v>717</v>
+      </c>
+      <c r="C163" t="s">
+        <v>742</v>
+      </c>
+      <c r="D163" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="B164" t="s">
+        <v>718</v>
+      </c>
+      <c r="C164" t="s">
+        <v>743</v>
+      </c>
+      <c r="D164" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="B165" t="s">
+        <v>726</v>
+      </c>
+      <c r="C165" t="s">
+        <v>744</v>
+      </c>
+      <c r="D165" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="B166" t="s">
+        <v>727</v>
+      </c>
+      <c r="C166" t="s">
+        <v>745</v>
+      </c>
+      <c r="D166" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="B167" t="s">
+        <v>728</v>
+      </c>
+      <c r="C167" t="s">
+        <v>746</v>
+      </c>
+      <c r="D167" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="B168" t="s">
+        <v>729</v>
+      </c>
+      <c r="C168" t="s">
+        <v>747</v>
+      </c>
+      <c r="D168" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="B169" t="s">
+        <v>729</v>
+      </c>
+      <c r="C169" t="s">
+        <v>748</v>
+      </c>
+      <c r="D169" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="B170" t="s">
+        <v>768</v>
+      </c>
+      <c r="C170" t="s">
+        <v>770</v>
+      </c>
+      <c r="D170" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="B171" t="s">
+        <v>768</v>
+      </c>
+      <c r="C171" t="s">
+        <v>771</v>
+      </c>
+      <c r="D171" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="B172" t="s">
+        <v>786</v>
+      </c>
+      <c r="C172" t="s">
+        <v>788</v>
+      </c>
+      <c r="D172" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="4" t="s">
+        <v>774</v>
+      </c>
+      <c r="B173" t="s">
+        <v>789</v>
+      </c>
+      <c r="C173" t="s">
+        <v>790</v>
+      </c>
+      <c r="D173" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="B174" t="s">
+        <v>792</v>
+      </c>
+      <c r="C174" t="s">
+        <v>793</v>
+      </c>
+      <c r="D174" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="B175" t="s">
+        <v>795</v>
+      </c>
+      <c r="C175" t="s">
+        <v>797</v>
+      </c>
+      <c r="D175" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="B176" t="s">
+        <v>795</v>
+      </c>
+      <c r="C176" t="s">
+        <v>799</v>
+      </c>
+      <c r="D176" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B177" t="s">
+        <v>800</v>
+      </c>
+      <c r="C177" t="s">
+        <v>790</v>
+      </c>
+      <c r="D177" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="C178" t="s">
+        <v>806</v>
+      </c>
+      <c r="D178" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="B179" t="s">
+        <v>802</v>
+      </c>
+      <c r="C179" t="s">
+        <v>805</v>
+      </c>
+      <c r="D179" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="B180" t="s">
+        <v>802</v>
+      </c>
+      <c r="C180" t="s">
+        <v>803</v>
+      </c>
+      <c r="D180" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="B181" t="s">
+        <v>808</v>
+      </c>
+      <c r="C181" t="s">
+        <v>810</v>
+      </c>
+      <c r="D181" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="B182" t="s">
+        <v>811</v>
+      </c>
+      <c r="C182" t="s">
+        <v>813</v>
+      </c>
+      <c r="D182" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="B183" t="s">
+        <v>814</v>
+      </c>
+      <c r="C183" t="s">
+        <v>815</v>
+      </c>
+      <c r="D183" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="B184" t="s">
+        <v>817</v>
+      </c>
+      <c r="C184" t="s">
+        <v>819</v>
+      </c>
+      <c r="D184" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="B185" t="s">
+        <v>820</v>
+      </c>
+      <c r="C185" t="s">
+        <v>822</v>
+      </c>
+      <c r="D185" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="B186" t="s">
+        <v>825</v>
+      </c>
+      <c r="C186" t="s">
+        <v>827</v>
+      </c>
+      <c r="D186" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="B187" t="s">
+        <v>828</v>
+      </c>
+      <c r="C187" t="s">
+        <v>829</v>
+      </c>
+      <c r="D187" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="B188" t="s">
+        <v>835</v>
+      </c>
+      <c r="C188" t="s">
+        <v>836</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="B189" t="s">
+        <v>838</v>
+      </c>
+      <c r="C189" t="s">
+        <v>840</v>
+      </c>
+      <c r="D189" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="B190" t="s">
+        <v>841</v>
+      </c>
+      <c r="C190" t="s">
+        <v>843</v>
+      </c>
+      <c r="D190" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="4" t="s">
+        <v>847</v>
+      </c>
+      <c r="B191" t="s">
+        <v>844</v>
+      </c>
+      <c r="C191" t="s">
+        <v>845</v>
+      </c>
+      <c r="D191" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="B192" t="s">
+        <v>849</v>
+      </c>
+      <c r="C192" t="s">
+        <v>850</v>
+      </c>
+      <c r="D192" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="4"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F45">

</xml_diff>